<commit_message>
Se actualiza el logo de la compañia en los forms
</commit_message>
<xml_diff>
--- a/SESTicket/SESTicket/Reports/xlsx/ticketecopetrol.xlsx
+++ b/SESTicket/SESTicket/Reports/xlsx/ticketecopetrol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdecou\Source\Repos\SESTicket\SESTicket\SESTicket\Reports\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RepositorioSesticket\SESTicket\SESTicket\Reports\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636E2427-C613-4983-B25A-A1DC88F52691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9007EE29-59F4-4E87-A55F-B00E02A7FD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS" sheetId="2" r:id="rId1"/>
@@ -629,7 +629,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy\ hh:mm"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1327,10 +1327,145 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1351,15 +1486,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1377,132 +1503,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1753,22 +1753,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>54429</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>503465</xdr:rowOff>
+      <xdr:colOff>428626</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>56336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1528082</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>429987</xdr:rowOff>
+      <xdr:colOff>1181650</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB25B5BF-5921-03ED-E9CB-3BB9A6FA50CF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1777,7 +1777,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1790,8 +1790,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1605643" y="2326822"/>
-          <a:ext cx="3038475" cy="838200"/>
+          <a:off x="2667001" y="3612336"/>
+          <a:ext cx="2356399" cy="1324789"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2099,23 +2099,23 @@
       <selection activeCell="B2" sqref="B2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="46.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="46.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" style="4" customWidth="1"/>
     <col min="7" max="7" width="42" style="4" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="40.85546875" style="4" customWidth="1"/>
-    <col min="10" max="11" width="24.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="3.42578125" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="4"/>
+    <col min="8" max="8" width="26.5546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="40.88671875" style="4" customWidth="1"/>
+    <col min="10" max="11" width="24.6640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="3.44140625" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2129,59 +2129,59 @@
       <c r="K1" s="2"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:12" ht="42" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="42" customHeight="1" thickTop="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="80" t="s">
+      <c r="B2" s="76"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="82"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="84"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="39" customHeight="1">
       <c r="A3" s="5"/>
-      <c r="B3" s="76"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="83" t="s">
+      <c r="B3" s="78"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="85" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="85"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="87"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="36" customHeight="1" thickBot="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="86" t="s">
+      <c r="B4" s="80"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="88" t="s">
         <v>184</v>
       </c>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="88" t="s">
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="90" t="s">
         <v>186</v>
       </c>
-      <c r="H4" s="89"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="87" t="s">
+      <c r="H4" s="91"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="K4" s="91"/>
+      <c r="K4" s="93"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="21" customHeight="1" thickTop="1">
       <c r="A5" s="5"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2195,29 +2195,29 @@
       <c r="K5" s="7"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="55.5" customHeight="1">
       <c r="A6" s="5"/>
-      <c r="B6" s="94"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="96"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="58"/>
       <c r="E6" s="7"/>
       <c r="F6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="71" t="s">
+      <c r="G6" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="72"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="95"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="5"/>
-      <c r="B7" s="97"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="99"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
       <c r="E7" s="7"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -2226,23 +2226,23 @@
       <c r="K7" s="8"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="35.1" customHeight="1">
       <c r="A8" s="5"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="100" t="s">
+      <c r="F8" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="62"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="64"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="18" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
@@ -2256,13 +2256,13 @@
       <c r="K9" s="15"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="35.1" customHeight="1">
       <c r="A10" s="5"/>
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="72" t="s">
         <v>174</v>
       </c>
-      <c r="C10" s="109"/>
-      <c r="D10" s="110"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="74"/>
       <c r="E10" s="7"/>
       <c r="F10" s="42" t="s">
         <v>25</v>
@@ -2280,11 +2280,11 @@
       <c r="K10" s="18"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="35.1" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="111"/>
-      <c r="C11" s="109"/>
-      <c r="D11" s="110"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="74"/>
       <c r="E11" s="7"/>
       <c r="F11" s="42" t="s">
         <v>27</v>
@@ -2298,11 +2298,11 @@
       <c r="K11" s="18"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="35.1" customHeight="1">
       <c r="A12" s="5"/>
-      <c r="B12" s="111"/>
-      <c r="C12" s="109"/>
-      <c r="D12" s="110"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="74"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -2312,41 +2312,41 @@
       <c r="K12" s="7"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="35.1" customHeight="1">
       <c r="A13" s="5"/>
-      <c r="B13" s="111"/>
-      <c r="C13" s="109"/>
-      <c r="D13" s="110"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="74"/>
       <c r="E13" s="7"/>
       <c r="F13" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="59" t="s">
+      <c r="G13" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="60"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
+      <c r="K13" s="105"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="35.1" customHeight="1">
       <c r="A14" s="5"/>
-      <c r="B14" s="111"/>
-      <c r="C14" s="109"/>
-      <c r="D14" s="110"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="74"/>
       <c r="E14" s="7"/>
       <c r="F14" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="62"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="64"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="35.1" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
@@ -2355,16 +2355,16 @@
       <c r="F15" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="96" t="s">
         <v>176</v>
       </c>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="63"/>
+      <c r="H15" s="96"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="97"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="35.1" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="21"/>
       <c r="C16" s="15"/>
@@ -2386,7 +2386,7 @@
       <c r="K16" s="22"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="35.25" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -2400,16 +2400,16 @@
       <c r="K17" s="24"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="42" customHeight="1">
       <c r="A18" s="5"/>
       <c r="B18" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="54"/>
-      <c r="E18" s="63"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="97"/>
       <c r="F18" s="43" t="s">
         <v>32</v>
       </c>
@@ -2419,23 +2419,23 @@
       <c r="H18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="53" t="s">
+      <c r="I18" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="J18" s="54"/>
-      <c r="K18" s="63"/>
+      <c r="J18" s="96"/>
+      <c r="K18" s="97"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="35.1" customHeight="1">
       <c r="A19" s="5"/>
       <c r="B19" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="54"/>
-      <c r="E19" s="63"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="97"/>
       <c r="F19" s="43" t="s">
         <v>10</v>
       </c>
@@ -2445,27 +2445,27 @@
       <c r="H19" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="I19" s="53" t="s">
+      <c r="I19" s="98" t="s">
         <v>182</v>
       </c>
-      <c r="J19" s="54"/>
-      <c r="K19" s="63"/>
+      <c r="J19" s="96"/>
+      <c r="K19" s="97"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="35.1" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="54"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="73" t="s">
+      <c r="D20" s="96"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="73"/>
+      <c r="G20" s="99"/>
       <c r="H20" s="26" t="s">
         <v>42</v>
       </c>
@@ -2474,7 +2474,7 @@
       <c r="K20" s="18"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="35.1" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -2488,16 +2488,16 @@
       <c r="K21" s="7"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="35.1" customHeight="1">
       <c r="A22" s="5"/>
       <c r="B22" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="54"/>
-      <c r="E22" s="63"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="97"/>
       <c r="F22" s="45" t="s">
         <v>31</v>
       </c>
@@ -2514,39 +2514,39 @@
       <c r="K22" s="18"/>
       <c r="L22" s="6"/>
     </row>
-    <row r="23" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="35.1" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="63"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="97"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="90" customHeight="1">
       <c r="A24" s="5"/>
-      <c r="B24" s="100"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="62"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="63"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="64"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="35.1" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
@@ -2560,20 +2560,20 @@
       <c r="K25" s="29"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="1:12" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="63.75" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="C26" s="64" t="s">
+      <c r="C26" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="66"/>
+      <c r="D26" s="107"/>
+      <c r="E26" s="107"/>
+      <c r="F26" s="107"/>
+      <c r="G26" s="107"/>
+      <c r="H26" s="107"/>
+      <c r="I26" s="108"/>
       <c r="J26" s="47" t="s">
         <v>20</v>
       </c>
@@ -2582,20 +2582,20 @@
       </c>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="32.1" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="70" t="s">
+      <c r="C27" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="70"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="70"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
       <c r="J27" s="33" t="s">
         <v>116</v>
       </c>
@@ -2604,20 +2604,20 @@
       </c>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="32.1" customHeight="1">
       <c r="A28" s="5"/>
       <c r="B28" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="70" t="s">
+      <c r="C28" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="70"/>
-      <c r="I28" s="70"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
       <c r="J28" s="33" t="s">
         <v>117</v>
       </c>
@@ -2626,20 +2626,20 @@
       </c>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="32.1" customHeight="1">
       <c r="A29" s="5"/>
       <c r="B29" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="70" t="s">
+      <c r="C29" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="70"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="70"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
       <c r="J29" s="33" t="s">
         <v>118</v>
       </c>
@@ -2648,20 +2648,20 @@
       </c>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="32.1" customHeight="1">
       <c r="A30" s="5"/>
       <c r="B30" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="70" t="s">
+      <c r="C30" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="70"/>
-      <c r="H30" s="70"/>
-      <c r="I30" s="70"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
       <c r="J30" s="33" t="s">
         <v>119</v>
       </c>
@@ -2670,20 +2670,20 @@
       </c>
       <c r="L30" s="6"/>
     </row>
-    <row r="31" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="32.1" customHeight="1">
       <c r="A31" s="5"/>
       <c r="B31" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="70" t="s">
+      <c r="C31" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="70"/>
-      <c r="I31" s="70"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
       <c r="J31" s="33" t="s">
         <v>120</v>
       </c>
@@ -2692,20 +2692,20 @@
       </c>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="32.1" customHeight="1">
       <c r="A32" s="5"/>
       <c r="B32" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="70" t="s">
+      <c r="C32" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="70"/>
-      <c r="H32" s="70"/>
-      <c r="I32" s="70"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
       <c r="J32" s="33" t="s">
         <v>121</v>
       </c>
@@ -2714,20 +2714,20 @@
       </c>
       <c r="L32" s="6"/>
     </row>
-    <row r="33" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="32.1" customHeight="1">
       <c r="A33" s="5"/>
       <c r="B33" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="70" t="s">
+      <c r="C33" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="70"/>
-      <c r="H33" s="70"/>
-      <c r="I33" s="70"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
       <c r="J33" s="33" t="s">
         <v>122</v>
       </c>
@@ -2736,20 +2736,20 @@
       </c>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="32.1" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="70" t="s">
+      <c r="C34" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
       <c r="J34" s="33" t="s">
         <v>123</v>
       </c>
@@ -2758,20 +2758,20 @@
       </c>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="32.1" customHeight="1">
       <c r="A35" s="5"/>
       <c r="B35" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="70" t="s">
+      <c r="C35" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
       <c r="J35" s="33" t="s">
         <v>124</v>
       </c>
@@ -2780,20 +2780,20 @@
       </c>
       <c r="L35" s="6"/>
     </row>
-    <row r="36" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="32.1" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="70" t="s">
+      <c r="C36" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="70"/>
-      <c r="G36" s="70"/>
-      <c r="H36" s="70"/>
-      <c r="I36" s="70"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="53"/>
       <c r="J36" s="33" t="s">
         <v>65</v>
       </c>
@@ -2802,20 +2802,20 @@
       </c>
       <c r="L36" s="6"/>
     </row>
-    <row r="37" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="32.1" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="70" t="s">
+      <c r="C37" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="70"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
       <c r="J37" s="33" t="s">
         <v>67</v>
       </c>
@@ -2824,20 +2824,20 @@
       </c>
       <c r="L37" s="6"/>
     </row>
-    <row r="38" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="32.1" customHeight="1">
       <c r="A38" s="5"/>
       <c r="B38" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="70" t="s">
+      <c r="C38" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="70"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="70"/>
-      <c r="H38" s="70"/>
-      <c r="I38" s="70"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
       <c r="J38" s="33" t="s">
         <v>69</v>
       </c>
@@ -2846,20 +2846,20 @@
       </c>
       <c r="L38" s="6"/>
     </row>
-    <row r="39" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="32.1" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="70" t="s">
+      <c r="C39" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="70"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="70"/>
-      <c r="G39" s="70"/>
-      <c r="H39" s="70"/>
-      <c r="I39" s="70"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="53"/>
       <c r="J39" s="33" t="s">
         <v>71</v>
       </c>
@@ -2868,20 +2868,20 @@
       </c>
       <c r="L39" s="6"/>
     </row>
-    <row r="40" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="32.1" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="70" t="s">
+      <c r="C40" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="D40" s="70"/>
-      <c r="E40" s="70"/>
-      <c r="F40" s="70"/>
-      <c r="G40" s="70"/>
-      <c r="H40" s="70"/>
-      <c r="I40" s="70"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
       <c r="J40" s="33" t="s">
         <v>73</v>
       </c>
@@ -2890,20 +2890,20 @@
       </c>
       <c r="L40" s="6"/>
     </row>
-    <row r="41" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="32.1" customHeight="1">
       <c r="A41" s="5"/>
       <c r="B41" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="70" t="s">
+      <c r="C41" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
-      <c r="H41" s="70"/>
-      <c r="I41" s="70"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="53"/>
       <c r="J41" s="33" t="s">
         <v>75</v>
       </c>
@@ -2912,20 +2912,20 @@
       </c>
       <c r="L41" s="6"/>
     </row>
-    <row r="42" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="32.1" customHeight="1">
       <c r="A42" s="5"/>
       <c r="B42" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="70" t="s">
+      <c r="C42" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="70"/>
-      <c r="H42" s="70"/>
-      <c r="I42" s="70"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
       <c r="J42" s="33" t="s">
         <v>77</v>
       </c>
@@ -2934,20 +2934,20 @@
       </c>
       <c r="L42" s="6"/>
     </row>
-    <row r="43" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="32.1" customHeight="1">
       <c r="A43" s="5"/>
       <c r="B43" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="70" t="s">
+      <c r="C43" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="70"/>
-      <c r="H43" s="70"/>
-      <c r="I43" s="70"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="53"/>
       <c r="J43" s="33" t="s">
         <v>79</v>
       </c>
@@ -2956,20 +2956,20 @@
       </c>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="32.1" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="70" t="s">
+      <c r="C44" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="70"/>
-      <c r="G44" s="70"/>
-      <c r="H44" s="70"/>
-      <c r="I44" s="70"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
       <c r="J44" s="33" t="s">
         <v>81</v>
       </c>
@@ -2978,20 +2978,20 @@
       </c>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="32.1" customHeight="1">
       <c r="A45" s="5"/>
       <c r="B45" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="70" t="s">
+      <c r="C45" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="70"/>
-      <c r="E45" s="70"/>
-      <c r="F45" s="70"/>
-      <c r="G45" s="70"/>
-      <c r="H45" s="70"/>
-      <c r="I45" s="70"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
       <c r="J45" s="33" t="s">
         <v>83</v>
       </c>
@@ -3000,20 +3000,20 @@
       </c>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="32.1" customHeight="1">
       <c r="A46" s="5"/>
       <c r="B46" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="70" t="s">
+      <c r="C46" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="70"/>
-      <c r="E46" s="70"/>
-      <c r="F46" s="70"/>
-      <c r="G46" s="70"/>
-      <c r="H46" s="70"/>
-      <c r="I46" s="70"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
       <c r="J46" s="33" t="s">
         <v>85</v>
       </c>
@@ -3022,20 +3022,20 @@
       </c>
       <c r="L46" s="6"/>
     </row>
-    <row r="47" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="32.1" customHeight="1">
       <c r="A47" s="5"/>
       <c r="B47" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="C47" s="70" t="s">
+      <c r="C47" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="D47" s="70"/>
-      <c r="E47" s="70"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70"/>
-      <c r="H47" s="70"/>
-      <c r="I47" s="70"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="53"/>
       <c r="J47" s="33" t="s">
         <v>136</v>
       </c>
@@ -3044,20 +3044,20 @@
       </c>
       <c r="L47" s="6"/>
     </row>
-    <row r="48" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="32.1" customHeight="1">
       <c r="A48" s="5"/>
       <c r="B48" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="C48" s="70" t="s">
+      <c r="C48" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="70"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="70"/>
-      <c r="G48" s="70"/>
-      <c r="H48" s="70"/>
-      <c r="I48" s="70"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="53"/>
       <c r="J48" s="33" t="s">
         <v>140</v>
       </c>
@@ -3066,20 +3066,20 @@
       </c>
       <c r="L48" s="6"/>
     </row>
-    <row r="49" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="32.1" customHeight="1">
       <c r="A49" s="5"/>
       <c r="B49" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="C49" s="70" t="s">
+      <c r="C49" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="D49" s="70"/>
-      <c r="E49" s="70"/>
-      <c r="F49" s="70"/>
-      <c r="G49" s="70"/>
-      <c r="H49" s="70"/>
-      <c r="I49" s="70"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="53"/>
       <c r="J49" s="33" t="s">
         <v>144</v>
       </c>
@@ -3088,20 +3088,20 @@
       </c>
       <c r="L49" s="6"/>
     </row>
-    <row r="50" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="32.1" customHeight="1">
       <c r="A50" s="5"/>
       <c r="B50" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="C50" s="70" t="s">
+      <c r="C50" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="D50" s="70"/>
-      <c r="E50" s="70"/>
-      <c r="F50" s="70"/>
-      <c r="G50" s="70"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="70"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
       <c r="J50" s="33" t="s">
         <v>148</v>
       </c>
@@ -3110,20 +3110,20 @@
       </c>
       <c r="L50" s="6"/>
     </row>
-    <row r="51" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="32.1" customHeight="1">
       <c r="A51" s="5"/>
       <c r="B51" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="C51" s="70" t="s">
+      <c r="C51" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="D51" s="70"/>
-      <c r="E51" s="70"/>
-      <c r="F51" s="70"/>
-      <c r="G51" s="70"/>
-      <c r="H51" s="70"/>
-      <c r="I51" s="70"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="53"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="53"/>
       <c r="J51" s="33" t="s">
         <v>152</v>
       </c>
@@ -3132,20 +3132,20 @@
       </c>
       <c r="L51" s="6"/>
     </row>
-    <row r="52" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="32.1" customHeight="1">
       <c r="A52" s="5"/>
       <c r="B52" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="C52" s="70" t="s">
+      <c r="C52" s="53" t="s">
         <v>155</v>
       </c>
-      <c r="D52" s="70"/>
-      <c r="E52" s="70"/>
-      <c r="F52" s="70"/>
-      <c r="G52" s="70"/>
-      <c r="H52" s="70"/>
-      <c r="I52" s="70"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="53"/>
       <c r="J52" s="33" t="s">
         <v>156</v>
       </c>
@@ -3154,20 +3154,20 @@
       </c>
       <c r="L52" s="6"/>
     </row>
-    <row r="53" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="32.1" customHeight="1">
       <c r="A53" s="5"/>
       <c r="B53" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="C53" s="70" t="s">
+      <c r="C53" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="D53" s="70"/>
-      <c r="E53" s="70"/>
-      <c r="F53" s="70"/>
-      <c r="G53" s="70"/>
-      <c r="H53" s="70"/>
-      <c r="I53" s="70"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="53"/>
+      <c r="I53" s="53"/>
       <c r="J53" s="33" t="s">
         <v>160</v>
       </c>
@@ -3176,20 +3176,20 @@
       </c>
       <c r="L53" s="6"/>
     </row>
-    <row r="54" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="32.1" customHeight="1">
       <c r="A54" s="5"/>
       <c r="B54" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="C54" s="70" t="s">
+      <c r="C54" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="D54" s="70"/>
-      <c r="E54" s="70"/>
-      <c r="F54" s="70"/>
-      <c r="G54" s="70"/>
-      <c r="H54" s="70"/>
-      <c r="I54" s="70"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53"/>
+      <c r="I54" s="53"/>
       <c r="J54" s="33" t="s">
         <v>164</v>
       </c>
@@ -3198,20 +3198,20 @@
       </c>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="32.1" customHeight="1">
       <c r="A55" s="5"/>
       <c r="B55" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="C55" s="70" t="s">
+      <c r="C55" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="D55" s="70"/>
-      <c r="E55" s="70"/>
-      <c r="F55" s="70"/>
-      <c r="G55" s="70"/>
-      <c r="H55" s="70"/>
-      <c r="I55" s="70"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="53"/>
+      <c r="I55" s="53"/>
       <c r="J55" s="33" t="s">
         <v>168</v>
       </c>
@@ -3220,20 +3220,20 @@
       </c>
       <c r="L55" s="6"/>
     </row>
-    <row r="56" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="32.1" customHeight="1">
       <c r="A56" s="5"/>
       <c r="B56" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="C56" s="70" t="s">
+      <c r="C56" s="53" t="s">
         <v>171</v>
       </c>
-      <c r="D56" s="70"/>
-      <c r="E56" s="70"/>
-      <c r="F56" s="70"/>
-      <c r="G56" s="70"/>
-      <c r="H56" s="70"/>
-      <c r="I56" s="70"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="53"/>
       <c r="J56" s="33" t="s">
         <v>172</v>
       </c>
@@ -3242,7 +3242,7 @@
       </c>
       <c r="L56" s="6"/>
     </row>
-    <row r="57" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="31.5" customHeight="1">
       <c r="A57" s="5"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -3253,17 +3253,17 @@
       <c r="K57" s="7"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="56.25" customHeight="1">
       <c r="A58" s="5"/>
-      <c r="B58" s="53" t="s">
+      <c r="B58" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="C58" s="54"/>
-      <c r="D58" s="54"/>
-      <c r="E58" s="54"/>
-      <c r="F58" s="54"/>
-      <c r="G58" s="54"/>
-      <c r="H58" s="54"/>
+      <c r="C58" s="96"/>
+      <c r="D58" s="96"/>
+      <c r="E58" s="96"/>
+      <c r="F58" s="96"/>
+      <c r="G58" s="96"/>
+      <c r="H58" s="96"/>
       <c r="I58" s="16" t="s">
         <v>179</v>
       </c>
@@ -3271,7 +3271,7 @@
       <c r="K58" s="48"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="78.75" customHeight="1">
       <c r="A59" s="5"/>
       <c r="B59" s="35"/>
       <c r="C59" s="36"/>
@@ -3285,117 +3285,117 @@
       <c r="K59" s="37"/>
       <c r="L59" s="6"/>
     </row>
-    <row r="60" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="21" customHeight="1">
       <c r="A60" s="5"/>
-      <c r="B60" s="105" t="s">
+      <c r="B60" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C60" s="106"/>
-      <c r="D60" s="106"/>
-      <c r="E60" s="106"/>
-      <c r="F60" s="106"/>
-      <c r="G60" s="106"/>
-      <c r="H60" s="106"/>
-      <c r="I60" s="106"/>
-      <c r="J60" s="106"/>
-      <c r="K60" s="107"/>
+      <c r="C60" s="70"/>
+      <c r="D60" s="70"/>
+      <c r="E60" s="70"/>
+      <c r="F60" s="70"/>
+      <c r="G60" s="70"/>
+      <c r="H60" s="70"/>
+      <c r="I60" s="70"/>
+      <c r="J60" s="70"/>
+      <c r="K60" s="71"/>
       <c r="L60" s="6"/>
     </row>
-    <row r="61" spans="1:12" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="81.75" customHeight="1">
       <c r="A61" s="5"/>
-      <c r="B61" s="101" t="s">
+      <c r="B61" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="C61" s="102"/>
-      <c r="D61" s="102"/>
-      <c r="E61" s="102"/>
-      <c r="F61" s="102"/>
-      <c r="G61" s="102"/>
-      <c r="H61" s="102"/>
-      <c r="I61" s="102"/>
-      <c r="J61" s="102"/>
-      <c r="K61" s="104"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="66"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="66"/>
+      <c r="I61" s="66"/>
+      <c r="J61" s="66"/>
+      <c r="K61" s="68"/>
       <c r="L61" s="6"/>
     </row>
-    <row r="62" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="20.25" customHeight="1">
       <c r="A62" s="5"/>
-      <c r="B62" s="105" t="s">
+      <c r="B62" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="C62" s="106"/>
-      <c r="D62" s="106"/>
-      <c r="E62" s="106"/>
-      <c r="F62" s="106"/>
-      <c r="G62" s="106"/>
-      <c r="H62" s="106"/>
-      <c r="I62" s="106"/>
-      <c r="J62" s="106"/>
-      <c r="K62" s="107"/>
+      <c r="C62" s="70"/>
+      <c r="D62" s="70"/>
+      <c r="E62" s="70"/>
+      <c r="F62" s="70"/>
+      <c r="G62" s="70"/>
+      <c r="H62" s="70"/>
+      <c r="I62" s="70"/>
+      <c r="J62" s="70"/>
+      <c r="K62" s="71"/>
       <c r="L62" s="6"/>
     </row>
-    <row r="63" spans="1:12" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="130.5" customHeight="1">
       <c r="A63" s="5"/>
-      <c r="B63" s="101" t="s">
+      <c r="B63" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="C63" s="102"/>
-      <c r="D63" s="102"/>
-      <c r="E63" s="103"/>
-      <c r="F63" s="103"/>
-      <c r="G63" s="103"/>
-      <c r="H63" s="102"/>
-      <c r="I63" s="102"/>
-      <c r="J63" s="102"/>
-      <c r="K63" s="104"/>
+      <c r="C63" s="66"/>
+      <c r="D63" s="66"/>
+      <c r="E63" s="67"/>
+      <c r="F63" s="67"/>
+      <c r="G63" s="67"/>
+      <c r="H63" s="66"/>
+      <c r="I63" s="66"/>
+      <c r="J63" s="66"/>
+      <c r="K63" s="68"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="35.1" customHeight="1">
       <c r="A64" s="5"/>
-      <c r="B64" s="93" t="s">
+      <c r="B64" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C64" s="93"/>
-      <c r="D64" s="93"/>
+      <c r="C64" s="55"/>
+      <c r="D64" s="55"/>
       <c r="E64" s="49"/>
       <c r="F64" s="50"/>
       <c r="G64" s="51"/>
-      <c r="H64" s="64" t="s">
+      <c r="H64" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="I64" s="65"/>
-      <c r="J64" s="65"/>
-      <c r="K64" s="66"/>
+      <c r="I64" s="107"/>
+      <c r="J64" s="107"/>
+      <c r="K64" s="108"/>
       <c r="L64" s="6"/>
     </row>
-    <row r="65" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="35.1" customHeight="1">
       <c r="A65" s="5"/>
       <c r="B65" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="67" t="s">
+      <c r="C65" s="109" t="s">
         <v>39</v>
       </c>
-      <c r="D65" s="67"/>
-      <c r="E65" s="92"/>
-      <c r="F65" s="92"/>
+      <c r="D65" s="109"/>
+      <c r="E65" s="54"/>
+      <c r="F65" s="54"/>
       <c r="G65" s="7"/>
       <c r="H65" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I65" s="68" t="s">
+      <c r="I65" s="110" t="s">
         <v>50</v>
       </c>
-      <c r="J65" s="68"/>
-      <c r="K65" s="69"/>
+      <c r="J65" s="110"/>
+      <c r="K65" s="111"/>
       <c r="L65" s="6"/>
     </row>
-    <row r="66" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="35.1" customHeight="1">
       <c r="A66" s="5"/>
       <c r="B66" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="C66" s="55"/>
-      <c r="D66" s="56"/>
+      <c r="C66" s="100"/>
+      <c r="D66" s="101"/>
       <c r="E66" s="38"/>
       <c r="F66" s="38"/>
       <c r="G66" s="7"/>
@@ -3407,47 +3407,47 @@
       <c r="K66" s="41"/>
       <c r="L66" s="6"/>
     </row>
-    <row r="67" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="35.1" customHeight="1">
       <c r="A67" s="5"/>
       <c r="B67" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C67" s="67" t="s">
+      <c r="C67" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="D67" s="67"/>
-      <c r="E67" s="92"/>
-      <c r="F67" s="92"/>
+      <c r="D67" s="109"/>
+      <c r="E67" s="54"/>
+      <c r="F67" s="54"/>
       <c r="G67" s="7"/>
       <c r="H67" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I67" s="68" t="s">
+      <c r="I67" s="110" t="s">
         <v>49</v>
       </c>
-      <c r="J67" s="68"/>
-      <c r="K67" s="69"/>
+      <c r="J67" s="110"/>
+      <c r="K67" s="111"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="35.1" customHeight="1">
       <c r="A68" s="5"/>
       <c r="B68" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C68" s="67"/>
-      <c r="D68" s="67"/>
-      <c r="E68" s="92"/>
-      <c r="F68" s="92"/>
+      <c r="C68" s="109"/>
+      <c r="D68" s="109"/>
+      <c r="E68" s="54"/>
+      <c r="F68" s="54"/>
       <c r="G68" s="7"/>
       <c r="H68" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="I68" s="68"/>
-      <c r="J68" s="68"/>
-      <c r="K68" s="69"/>
+      <c r="I68" s="110"/>
+      <c r="J68" s="110"/>
+      <c r="K68" s="111"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" spans="1:12" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" ht="21" customHeight="1" thickBot="1">
       <c r="A69" s="5"/>
       <c r="B69" s="24"/>
       <c r="C69" s="24"/>
@@ -3461,31 +3461,72 @@
       <c r="K69" s="24"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" spans="1:12" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" ht="43.5" customHeight="1" thickBot="1">
       <c r="A70" s="39"/>
-      <c r="B70" s="57" t="s">
+      <c r="B70" s="102" t="s">
         <v>181</v>
       </c>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
-      <c r="F70" s="58"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="58"/>
-      <c r="I70" s="58"/>
-      <c r="J70" s="58"/>
-      <c r="K70" s="58"/>
+      <c r="C70" s="103"/>
+      <c r="D70" s="103"/>
+      <c r="E70" s="103"/>
+      <c r="F70" s="103"/>
+      <c r="G70" s="103"/>
+      <c r="H70" s="103"/>
+      <c r="I70" s="103"/>
+      <c r="J70" s="103"/>
+      <c r="K70" s="103"/>
       <c r="L70" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="C55:I55"/>
-    <mergeCell ref="C50:I50"/>
-    <mergeCell ref="C51:I51"/>
-    <mergeCell ref="C52:I52"/>
-    <mergeCell ref="C53:I53"/>
-    <mergeCell ref="C54:I54"/>
+    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="B70:K70"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="H64:K64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="I65:K65"/>
+    <mergeCell ref="I67:K67"/>
+    <mergeCell ref="I68:K68"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C23:K23"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B2:C4"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C56:I56"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="C42:I42"/>
+    <mergeCell ref="C43:I43"/>
+    <mergeCell ref="C44:I44"/>
+    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C37:I37"/>
+    <mergeCell ref="C38:I38"/>
+    <mergeCell ref="C46:I46"/>
+    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="C48:I48"/>
+    <mergeCell ref="C49:I49"/>
     <mergeCell ref="E68:F68"/>
     <mergeCell ref="E65:F65"/>
     <mergeCell ref="B64:D64"/>
@@ -3502,54 +3543,13 @@
     <mergeCell ref="F8:K8"/>
     <mergeCell ref="C33:I33"/>
     <mergeCell ref="B10:D14"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C56:I56"/>
-    <mergeCell ref="C41:I41"/>
-    <mergeCell ref="C42:I42"/>
-    <mergeCell ref="C43:I43"/>
-    <mergeCell ref="C44:I44"/>
-    <mergeCell ref="C45:I45"/>
-    <mergeCell ref="C37:I37"/>
-    <mergeCell ref="C38:I38"/>
-    <mergeCell ref="C46:I46"/>
-    <mergeCell ref="C47:I47"/>
-    <mergeCell ref="C48:I48"/>
-    <mergeCell ref="C49:I49"/>
-    <mergeCell ref="B2:C4"/>
-    <mergeCell ref="D2:K2"/>
-    <mergeCell ref="D3:K3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C23:K23"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="B58:H58"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="B70:K70"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="H64:K64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="I65:K65"/>
-    <mergeCell ref="I67:K67"/>
-    <mergeCell ref="I68:K68"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="C55:I55"/>
+    <mergeCell ref="C50:I50"/>
+    <mergeCell ref="C51:I51"/>
+    <mergeCell ref="C52:I52"/>
+    <mergeCell ref="C53:I53"/>
+    <mergeCell ref="C54:I54"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.35" bottom="0.32" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>